<commit_message>
working on diet data from cages and smelt recapgure data
</commit_message>
<xml_diff>
--- a/data/Running Delta Smelt Catch.xlsx
+++ b/data/Running Delta Smelt Catch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/smelt cages/Smelt-cages/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{D9C32DC8-52D0-4672-8A87-DE64BFFD741D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4DC517C-8907-4689-B551-9395E1749399}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{D9C32DC8-52D0-4672-8A87-DE64BFFD741D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{479E2EDD-7A78-432A-99E6-6788A38388E2}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="1" xr2:uid="{4BB403AD-DB3F-4CB5-B7F1-39827ED458E8}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3468" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3559" uniqueCount="502">
   <si>
     <t>Running Delta Smelt Catch Data Collected for the USFWS Delta Smelt Experimental Release Technical Team</t>
   </si>
@@ -1527,6 +1527,45 @@
   </si>
   <si>
     <t>Dateknown</t>
+  </si>
+  <si>
+    <t>24-33-SM02</t>
+  </si>
+  <si>
+    <t>S261</t>
+  </si>
+  <si>
+    <t>24-33-SSC03</t>
+  </si>
+  <si>
+    <t>S332</t>
+  </si>
+  <si>
+    <t>24-33-LSR02</t>
+  </si>
+  <si>
+    <t>S333</t>
+  </si>
+  <si>
+    <t>24-35-LSR02</t>
+  </si>
+  <si>
+    <t>S334</t>
+  </si>
+  <si>
+    <t>24-35-SM03</t>
+  </si>
+  <si>
+    <t>S262</t>
+  </si>
+  <si>
+    <t>S263</t>
+  </si>
+  <si>
+    <t>24-35-SSC03</t>
+  </si>
+  <si>
+    <t>S335</t>
   </si>
 </sst>
 </file>
@@ -1536,7 +1575,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1607,6 +1646,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1680,7 +1725,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1773,6 +1818,16 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2485,11 +2540,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C569B310-60E0-4E31-89EB-52CC1C810311}">
-  <dimension ref="A1:AE255"/>
+  <dimension ref="A1:AE262"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J227" sqref="J227"/>
+      <pane ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H270" sqref="H270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -18890,7 +18945,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="241" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A241" s="20">
         <v>45335</v>
       </c>
@@ -18959,7 +19014,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="242" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A242" s="20">
         <v>45336</v>
       </c>
@@ -19028,7 +19083,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="243" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A243" s="20">
         <v>45336</v>
       </c>
@@ -19097,7 +19152,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="244" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A244" s="20">
         <v>45336</v>
       </c>
@@ -19166,7 +19221,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="245" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A245" s="20">
         <v>45339</v>
       </c>
@@ -19223,7 +19278,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="246" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A246" s="20">
         <v>45339</v>
       </c>
@@ -19280,7 +19335,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="247" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A247" s="20">
         <v>45340</v>
       </c>
@@ -19337,7 +19392,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="248" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A248" s="20">
         <v>45340</v>
       </c>
@@ -19394,7 +19449,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="249" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A249" s="20">
         <v>45344</v>
       </c>
@@ -19451,7 +19506,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="250" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A250" s="20">
         <v>45345</v>
       </c>
@@ -19505,7 +19560,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="251" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A251" s="20">
         <v>45345</v>
       </c>
@@ -19559,7 +19614,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="252" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A252" s="20">
         <v>45348</v>
       </c>
@@ -19628,7 +19683,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="253" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A253" s="20">
         <v>45349</v>
       </c>
@@ -19697,7 +19752,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="254" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A254" s="20">
         <v>45350</v>
       </c>
@@ -19766,7 +19821,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="255" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A255" s="20">
         <v>45350</v>
       </c>
@@ -19834,6 +19889,545 @@
       <c r="W255" s="14" t="s">
         <v>439</v>
       </c>
+    </row>
+    <row r="256" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A256" s="37">
+        <v>45362</v>
+      </c>
+      <c r="B256" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="C256" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="D256" s="31" t="s">
+        <v>489</v>
+      </c>
+      <c r="E256" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="F256" s="31">
+        <v>1113</v>
+      </c>
+      <c r="G256" s="31">
+        <v>13.5</v>
+      </c>
+      <c r="H256" s="31">
+        <v>70.2</v>
+      </c>
+      <c r="I256" s="31">
+        <v>47.32</v>
+      </c>
+      <c r="J256" s="31">
+        <v>72</v>
+      </c>
+      <c r="K256" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="L256" s="31">
+        <v>38.146929999999998</v>
+      </c>
+      <c r="M256" s="31">
+        <v>-122.05933</v>
+      </c>
+      <c r="N256" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="O256" s="31" t="s">
+        <v>490</v>
+      </c>
+      <c r="P256" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q256" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="R256" s="31" t="s">
+        <v>426</v>
+      </c>
+      <c r="S256" s="31" t="s">
+        <v>427</v>
+      </c>
+      <c r="T256" s="37">
+        <v>45315</v>
+      </c>
+      <c r="U256" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="V256" s="31" t="s">
+        <v>428</v>
+      </c>
+      <c r="W256" s="31"/>
+      <c r="X256" s="40"/>
+      <c r="Y256" s="39"/>
+      <c r="Z256" s="39"/>
+      <c r="AA256" s="39"/>
+      <c r="AB256" s="39"/>
+      <c r="AC256" s="39"/>
+      <c r="AD256" s="39"/>
+      <c r="AE256" s="39"/>
+    </row>
+    <row r="257" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A257" s="37">
+        <v>45362</v>
+      </c>
+      <c r="B257" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="C257" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="D257" s="31" t="s">
+        <v>491</v>
+      </c>
+      <c r="E257" s="31" t="s">
+        <v>422</v>
+      </c>
+      <c r="F257" s="31">
+        <v>334.2</v>
+      </c>
+      <c r="G257" s="31">
+        <v>12.6</v>
+      </c>
+      <c r="H257" s="31">
+        <v>55.9</v>
+      </c>
+      <c r="I257" s="31">
+        <v>34.11</v>
+      </c>
+      <c r="J257" s="31">
+        <v>66</v>
+      </c>
+      <c r="K257" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="L257" s="31">
+        <v>38.289020000000001</v>
+      </c>
+      <c r="M257" s="31">
+        <v>-121.65742</v>
+      </c>
+      <c r="N257" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="O257" s="31" t="s">
+        <v>492</v>
+      </c>
+      <c r="P257" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q257" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="R257" s="31" t="s">
+        <v>480</v>
+      </c>
+      <c r="S257" s="31" t="s">
+        <v>481</v>
+      </c>
+      <c r="T257" s="37">
+        <v>45274</v>
+      </c>
+      <c r="U257" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="V257" s="31" t="s">
+        <v>439</v>
+      </c>
+      <c r="W257" s="31"/>
+      <c r="X257" s="40"/>
+      <c r="Y257" s="39"/>
+      <c r="Z257" s="39"/>
+      <c r="AA257" s="39"/>
+      <c r="AB257" s="39"/>
+      <c r="AC257" s="39"/>
+      <c r="AD257" s="39"/>
+      <c r="AE257" s="39"/>
+    </row>
+    <row r="258" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A258" s="37">
+        <v>45364</v>
+      </c>
+      <c r="B258" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="C258" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="D258" s="31" t="s">
+        <v>493</v>
+      </c>
+      <c r="E258" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="F258" s="31">
+        <v>195.3</v>
+      </c>
+      <c r="G258" s="31">
+        <v>12.1</v>
+      </c>
+      <c r="H258" s="31">
+        <v>43.5</v>
+      </c>
+      <c r="I258" s="31">
+        <v>22.53</v>
+      </c>
+      <c r="J258" s="31">
+        <v>79</v>
+      </c>
+      <c r="K258" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="L258" s="31">
+        <v>38.064660000000003</v>
+      </c>
+      <c r="M258" s="31">
+        <v>-121.79474999999999</v>
+      </c>
+      <c r="N258" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="O258" s="31" t="s">
+        <v>494</v>
+      </c>
+      <c r="P258" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q258" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="R258" s="31" t="s">
+        <v>437</v>
+      </c>
+      <c r="S258" s="31" t="s">
+        <v>438</v>
+      </c>
+      <c r="T258" s="37">
+        <v>45316</v>
+      </c>
+      <c r="U258" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="V258" s="31" t="s">
+        <v>439</v>
+      </c>
+      <c r="W258" s="31"/>
+      <c r="X258" s="40"/>
+      <c r="Y258" s="39"/>
+      <c r="Z258" s="39"/>
+      <c r="AA258" s="39"/>
+      <c r="AB258" s="39"/>
+      <c r="AC258" s="39"/>
+      <c r="AD258" s="39"/>
+      <c r="AE258" s="39"/>
+    </row>
+    <row r="259" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A259" s="37">
+        <v>45376</v>
+      </c>
+      <c r="B259" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="C259" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="D259" s="31" t="s">
+        <v>495</v>
+      </c>
+      <c r="E259" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="F259" s="31">
+        <v>199.9</v>
+      </c>
+      <c r="G259" s="31">
+        <v>14.2</v>
+      </c>
+      <c r="H259" s="31">
+        <v>26.6</v>
+      </c>
+      <c r="I259" s="31">
+        <v>15.37</v>
+      </c>
+      <c r="J259" s="31">
+        <v>76</v>
+      </c>
+      <c r="K259" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="L259" s="31">
+        <v>38.06373</v>
+      </c>
+      <c r="M259" s="31">
+        <v>-121.81019999999999</v>
+      </c>
+      <c r="N259" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="O259" s="31" t="s">
+        <v>496</v>
+      </c>
+      <c r="P259" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q259" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="R259" s="31" t="s">
+        <v>426</v>
+      </c>
+      <c r="S259" s="31" t="s">
+        <v>427</v>
+      </c>
+      <c r="T259" s="37">
+        <v>45315</v>
+      </c>
+      <c r="U259" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="V259" s="31" t="s">
+        <v>428</v>
+      </c>
+      <c r="W259" s="31"/>
+      <c r="X259" s="40"/>
+      <c r="Y259" s="39"/>
+      <c r="Z259" s="39"/>
+      <c r="AA259" s="39"/>
+      <c r="AB259" s="39"/>
+      <c r="AC259" s="39"/>
+      <c r="AD259" s="39"/>
+      <c r="AE259" s="39"/>
+    </row>
+    <row r="260" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A260" s="37">
+        <v>45376</v>
+      </c>
+      <c r="B260" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="C260" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="D260" s="31" t="s">
+        <v>497</v>
+      </c>
+      <c r="E260" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="F260" s="31">
+        <v>864</v>
+      </c>
+      <c r="G260" s="31">
+        <v>15.1</v>
+      </c>
+      <c r="H260" s="31">
+        <v>45.3</v>
+      </c>
+      <c r="I260" s="31">
+        <v>28.32</v>
+      </c>
+      <c r="J260" s="31">
+        <v>85</v>
+      </c>
+      <c r="K260" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="L260" s="31">
+        <v>38.186950000000003</v>
+      </c>
+      <c r="M260" s="31">
+        <v>-121.97835000000001</v>
+      </c>
+      <c r="N260" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="O260" s="31" t="s">
+        <v>498</v>
+      </c>
+      <c r="P260" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q260" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="R260" s="31" t="s">
+        <v>426</v>
+      </c>
+      <c r="S260" s="31" t="s">
+        <v>427</v>
+      </c>
+      <c r="T260" s="37">
+        <v>45315</v>
+      </c>
+      <c r="U260" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="V260" s="31" t="s">
+        <v>428</v>
+      </c>
+      <c r="W260" s="31"/>
+      <c r="X260" s="40"/>
+      <c r="Y260" s="39"/>
+      <c r="Z260" s="39"/>
+      <c r="AA260" s="39"/>
+      <c r="AB260" s="39"/>
+      <c r="AC260" s="39"/>
+      <c r="AD260" s="39"/>
+      <c r="AE260" s="39"/>
+    </row>
+    <row r="261" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A261" s="37">
+        <v>45376</v>
+      </c>
+      <c r="B261" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="C261" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="D261" s="31" t="s">
+        <v>497</v>
+      </c>
+      <c r="E261" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="F261" s="31">
+        <v>880</v>
+      </c>
+      <c r="G261" s="31">
+        <v>15.1</v>
+      </c>
+      <c r="H261" s="31">
+        <v>45.3</v>
+      </c>
+      <c r="I261" s="31">
+        <v>27.63</v>
+      </c>
+      <c r="J261" s="31">
+        <v>81</v>
+      </c>
+      <c r="K261" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="L261" s="31">
+        <v>38.186819999999997</v>
+      </c>
+      <c r="M261" s="31">
+        <v>-121.97931</v>
+      </c>
+      <c r="N261" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="O261" s="31" t="s">
+        <v>499</v>
+      </c>
+      <c r="P261" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q261" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="R261" s="31" t="s">
+        <v>426</v>
+      </c>
+      <c r="S261" s="31" t="s">
+        <v>427</v>
+      </c>
+      <c r="T261" s="37">
+        <v>45315</v>
+      </c>
+      <c r="U261" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="V261" s="31" t="s">
+        <v>428</v>
+      </c>
+      <c r="W261" s="31"/>
+      <c r="X261" s="40"/>
+      <c r="Y261" s="39"/>
+      <c r="Z261" s="39"/>
+      <c r="AA261" s="39"/>
+      <c r="AB261" s="39"/>
+      <c r="AC261" s="39"/>
+      <c r="AD261" s="39"/>
+      <c r="AE261" s="39"/>
+    </row>
+    <row r="262" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A262" s="37">
+        <v>45377</v>
+      </c>
+      <c r="B262" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="C262" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="D262" s="31" t="s">
+        <v>500</v>
+      </c>
+      <c r="E262" s="31" t="s">
+        <v>422</v>
+      </c>
+      <c r="F262" s="31">
+        <v>630</v>
+      </c>
+      <c r="G262" s="31">
+        <v>15</v>
+      </c>
+      <c r="H262" s="31">
+        <v>30.5</v>
+      </c>
+      <c r="I262" s="31">
+        <v>18.87</v>
+      </c>
+      <c r="J262" s="31">
+        <v>61</v>
+      </c>
+      <c r="K262" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="L262" s="31">
+        <v>38.314129999999999</v>
+      </c>
+      <c r="M262" s="31">
+        <v>-121.65241</v>
+      </c>
+      <c r="N262" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="O262" s="31" t="s">
+        <v>501</v>
+      </c>
+      <c r="P262" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q262" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="R262" s="31" t="s">
+        <v>480</v>
+      </c>
+      <c r="S262" s="31" t="s">
+        <v>481</v>
+      </c>
+      <c r="T262" s="37">
+        <v>45274</v>
+      </c>
+      <c r="U262" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="V262" s="31" t="s">
+        <v>439</v>
+      </c>
+      <c r="W262" s="31"/>
+      <c r="X262" s="40"/>
+      <c r="Y262" s="39"/>
+      <c r="Z262" s="39"/>
+      <c r="AA262" s="39"/>
+      <c r="AB262" s="39"/>
+      <c r="AC262" s="39"/>
+      <c r="AD262" s="39"/>
+      <c r="AE262" s="39"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AE255" xr:uid="{C569B310-60E0-4E31-89EB-52CC1C810311}">
@@ -19858,36 +20452,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="65146633-a755-433a-aacb-5024b6511b89">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d8e23be6-d007-4c2c-9265-7d9405abf22e" xsi:nil="true"/>
-    <SharedWithUsers xmlns="d8e23be6-d007-4c2c-9265-7d9405abf22e">
-      <UserInfo>
-        <DisplayName>Hartman, Rosemary@DWR</DisplayName>
-        <AccountId>69</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Goodman, Denise M</DisplayName>
-        <AccountId>31</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Hobbs, James@Wildlife</DisplayName>
-        <AccountId>16</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Cook, John (Ryan)</DisplayName>
-        <AccountId>18</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20126,21 +20696,42 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="65146633-a755-433a-aacb-5024b6511b89">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d8e23be6-d007-4c2c-9265-7d9405abf22e" xsi:nil="true"/>
+    <SharedWithUsers xmlns="d8e23be6-d007-4c2c-9265-7d9405abf22e">
+      <UserInfo>
+        <DisplayName>Hartman, Rosemary@DWR</DisplayName>
+        <AccountId>69</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Goodman, Denise M</DisplayName>
+        <AccountId>31</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Hobbs, James@Wildlife</DisplayName>
+        <AccountId>16</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Cook, John (Ryan)</DisplayName>
+        <AccountId>18</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D4F8AF6-B64B-4962-81B5-D73EE7A1E0CA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7C764E5-19B4-4012-98BF-B46F2FA7A2CF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="65146633-a755-433a-aacb-5024b6511b89"/>
-    <ds:schemaRef ds:uri="d8e23be6-d007-4c2c-9265-7d9405abf22e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -20165,9 +20756,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7C764E5-19B4-4012-98BF-B46F2FA7A2CF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D4F8AF6-B64B-4962-81B5-D73EE7A1E0CA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="65146633-a755-433a-aacb-5024b6511b89"/>
+    <ds:schemaRef ds:uri="d8e23be6-d007-4c2c-9265-7d9405abf22e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>